<commit_message>
Adding corporate tax rate
</commit_message>
<xml_diff>
--- a/FinancialManagement/Pharma_Data.xlsx
+++ b/FinancialManagement/Pharma_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goomb\Documents\Datasets\FinancialManagement\Pharma_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB63AA8-9CE7-4FA3-9C92-646F8CD9E602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE7DB7C-C080-4BB2-8A92-1D4A7BD45BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Search strategy" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,98 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={6D7E679E-BD2F-441B-88DC-4231C8BC6A1C}</author>
+  </authors>
+  <commentList>
+    <comment ref="Q11" authorId="0" shapeId="0" xr:uid="{6D7E679E-BD2F-441B-88DC-4231C8BC6A1C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    9% del Estado de Nueva Jersey y 21% federal de EEUU</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={04297985-960D-4A6D-B72C-D25F288EBCA2}</author>
+  </authors>
+  <commentList>
+    <comment ref="Q11" authorId="0" shapeId="0" xr:uid="{04297985-960D-4A6D-B72C-D25F288EBCA2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    15% es el máximo en la región de Basilea en Suiza</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={427EB58A-84ED-4BA1-BFBD-2D82CABA1FF1}</author>
+  </authors>
+  <commentList>
+    <comment ref="Q11" authorId="0" shapeId="0" xr:uid="{427EB58A-84ED-4BA1-BFBD-2D82CABA1FF1}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    7,25% del Estad de Nueva York y 21% federal
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D1CB7C83-2261-4BA5-9694-B0C208C79A51}</author>
+  </authors>
+  <commentList>
+    <comment ref="Q11" authorId="0" shapeId="0" xr:uid="{D1CB7C83-2261-4BA5-9694-B0C208C79A51}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    15% es el tipo corporativo máximo en Basilea, Suiza</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={52883D57-F86C-480B-9960-F09CA44D92A4}</author>
+  </authors>
+  <commentList>
+    <comment ref="Q11" authorId="0" shapeId="0" xr:uid="{52883D57-F86C-480B-9960-F09CA44D92A4}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    8,5% del estado de Indiana y 21% tipo federal de EEUU
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="199">
   <si>
@@ -955,14 +1047,14 @@
     <t>D</t>
   </si>
   <si>
-    <t>Effective Tax rate</t>
+    <t>t_c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -996,6 +1088,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1096,7 +1194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1167,11 +1265,19 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1181,14 +1287,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,6 +1304,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Lucas Senande López" id="{D102DFAF-7AB4-4E26-AD3A-9DDD4F90D851}" userId="S::100473028@alumnos.uc3m.es::31d0fb0c-afe5-479c-baf8-21196e965742" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1521,6 +1627,48 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q11" dT="2024-04-16T20:44:33.13" personId="{D102DFAF-7AB4-4E26-AD3A-9DDD4F90D851}" id="{6D7E679E-BD2F-441B-88DC-4231C8BC6A1C}">
+    <text>9% del Estado de Nueva Jersey y 21% federal de EEUU</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q11" dT="2024-04-16T20:44:09.85" personId="{D102DFAF-7AB4-4E26-AD3A-9DDD4F90D851}" id="{04297985-960D-4A6D-B72C-D25F288EBCA2}">
+    <text>15% es el máximo en la región de Basilea en Suiza</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q11" dT="2024-04-16T20:45:44.09" personId="{D102DFAF-7AB4-4E26-AD3A-9DDD4F90D851}" id="{427EB58A-84ED-4BA1-BFBD-2D82CABA1FF1}">
+    <text xml:space="preserve">7,25% del Estad de Nueva York y 21% federal
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q11" dT="2024-04-16T20:46:36.72" personId="{D102DFAF-7AB4-4E26-AD3A-9DDD4F90D851}" id="{D1CB7C83-2261-4BA5-9694-B0C208C79A51}">
+    <text>15% es el tipo corporativo máximo en Basilea, Suiza</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q11" dT="2024-04-16T20:47:42.10" personId="{D102DFAF-7AB4-4E26-AD3A-9DDD4F90D851}" id="{52883D57-F86C-480B-9960-F09CA44D92A4}">
+    <text xml:space="preserve">8,5% del estado de Indiana y 21% tipo federal de EEUU
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
@@ -1540,86 +1688,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="33" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="34"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="34"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="34"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="34"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="34"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="33" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="34"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="33" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="34"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1631,10 +1779,10 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1646,10 +1794,10 @@
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1661,10 +1809,10 @@
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
@@ -1676,10 +1824,10 @@
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="26"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1691,10 +1839,10 @@
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="7" t="s">
         <v>18</v>
       </c>
@@ -1703,17 +1851,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="9" t="s">
         <v>33</v>
       </c>
@@ -1722,42 +1870,25 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="B11:C11"/>
@@ -1765,6 +1896,23 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4430,12 +4578,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03140F42-7C75-4C7D-9199-1DB0B1072644}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03140F42-7C75-4C7D-9199-1DB0B1072644}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4449,12 +4597,11 @@
     <col min="10" max="10" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>196</v>
       </c>
@@ -4501,13 +4648,13 @@
         <v>195</v>
       </c>
       <c r="P1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q1" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2014</v>
       </c>
@@ -4554,14 +4701,11 @@
         <v>3895000</v>
       </c>
       <c r="P2">
-        <v>0.25975617227225389</v>
-      </c>
-      <c r="Q2">
         <v>18760000</v>
       </c>
-      <c r="S2" s="25"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R2" s="25"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -4608,14 +4752,11 @@
         <v>3746000</v>
       </c>
       <c r="P3">
-        <v>0.24576546174313707</v>
-      </c>
-      <c r="Q3">
         <v>19861000</v>
       </c>
-      <c r="S3" s="25"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R3" s="25"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2016</v>
       </c>
@@ -4663,14 +4804,11 @@
         <v>3754000</v>
       </c>
       <c r="P4">
-        <v>0.19727932285368799</v>
-      </c>
-      <c r="Q4">
         <v>27126000</v>
       </c>
-      <c r="S4" s="25"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R4" s="25"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2017</v>
       </c>
@@ -4717,14 +4855,11 @@
         <v>5642000</v>
       </c>
       <c r="P5">
-        <v>12.594615384615384</v>
-      </c>
-      <c r="Q5">
         <v>34581000</v>
       </c>
-      <c r="S5" s="25"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R5" s="25"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -4771,14 +4906,11 @@
         <v>6929000</v>
       </c>
       <c r="P6">
-        <v>0.17663594168791263</v>
-      </c>
-      <c r="Q6">
         <v>29981000</v>
       </c>
-      <c r="S6" s="25"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R6" s="25"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2019</v>
       </c>
@@ -4825,14 +4957,11 @@
         <v>7009000</v>
       </c>
       <c r="P7">
-        <v>0.14610754679542293</v>
-      </c>
-      <c r="Q7">
         <v>27696000</v>
       </c>
-      <c r="S7" s="25"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R7" s="25"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -4879,14 +5008,11 @@
         <v>7300000</v>
       </c>
       <c r="P8">
-        <v>0.12117711023515021</v>
-      </c>
-      <c r="Q8">
         <v>35266000</v>
       </c>
-      <c r="S8" s="25"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R8" s="25"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -4933,14 +5059,11 @@
         <v>7390000</v>
       </c>
       <c r="P9">
-        <v>-8.1425423891177351E-2</v>
-      </c>
-      <c r="Q9">
         <v>33751000</v>
       </c>
-      <c r="S9" s="25"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R9" s="25"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -4988,14 +5111,11 @@
         <v>6970000</v>
       </c>
       <c r="P10">
-        <v>7.9036842985340749E-2</v>
-      </c>
-      <c r="Q10">
         <v>39659000</v>
       </c>
-      <c r="S10" s="25"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R10" s="25"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2023</v>
       </c>
@@ -5042,25 +5162,27 @@
         <v>7103000</v>
       </c>
       <c r="P11">
-        <v>-0.57153016812220869</v>
-      </c>
-      <c r="Q11">
         <v>29332000</v>
       </c>
-      <c r="S11" s="25"/>
+      <c r="Q11" s="36">
+        <f>9% + 21%</f>
+        <v>0.3</v>
+      </c>
+      <c r="R11" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D143F43-DDA8-48B7-AA53-77749AB56B8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D143F43-DDA8-48B7-AA53-77749AB56B8E}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5072,9 +5194,7 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -5124,10 +5244,10 @@
         <v>195</v>
       </c>
       <c r="P1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q1" t="s">
         <v>198</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -5177,9 +5297,6 @@
         <v>4632493.93486977</v>
       </c>
       <c r="P2">
-        <v>0.34108444063437782</v>
-      </c>
-      <c r="Q2">
         <v>25997369.934797198</v>
       </c>
     </row>
@@ -5230,9 +5347,6 @@
         <v>3931055.4742813101</v>
       </c>
       <c r="P3">
-        <v>0.35247658806273785</v>
-      </c>
-      <c r="Q3">
         <v>23436146.36731109</v>
       </c>
     </row>
@@ -5283,9 +5397,6 @@
         <v>5649606.3423156701</v>
       </c>
       <c r="P4">
-        <v>0.35829156223893222</v>
-      </c>
-      <c r="Q4">
         <v>22002952.923774719</v>
       </c>
     </row>
@@ -5336,9 +5447,6 @@
         <v>7831436.4495277395</v>
       </c>
       <c r="P5">
-        <v>0.41874203637206198</v>
-      </c>
-      <c r="Q5">
         <v>19440172.176361114</v>
       </c>
     </row>
@@ -5389,9 +5497,6 @@
         <v>7172743.0491447402</v>
       </c>
       <c r="P6">
-        <v>0.34742857142857386</v>
-      </c>
-      <c r="Q6">
         <v>19061643.357277006</v>
       </c>
     </row>
@@ -5442,9 +5547,6 @@
         <v>6516215.4725789996</v>
       </c>
       <c r="P7">
-        <v>0.23094020893531764</v>
-      </c>
-      <c r="Q7">
         <v>16093781.818628192</v>
       </c>
     </row>
@@ -5495,9 +5597,6 @@
         <v>5911257.4281692496</v>
       </c>
       <c r="P8">
-        <v>0.25673312346974586</v>
-      </c>
-      <c r="Q8">
         <v>17488651.991844594</v>
       </c>
     </row>
@@ -5548,9 +5647,6 @@
         <v>5583434.0066909799</v>
       </c>
       <c r="P9">
-        <v>0.24895908111988208</v>
-      </c>
-      <c r="Q9">
         <v>35665609.063148677</v>
       </c>
     </row>
@@ -5601,9 +5697,6 @@
         <v>7375033.8071584702</v>
       </c>
       <c r="P10">
-        <v>0.31446743418404499</v>
-      </c>
-      <c r="Q10">
         <v>28750609.102248698</v>
       </c>
     </row>
@@ -5654,23 +5747,26 @@
         <v>5643711.85350418</v>
       </c>
       <c r="P11">
-        <v>0.22447382153417794</v>
-      </c>
-      <c r="Q11">
         <v>36643058.062552899</v>
+      </c>
+      <c r="Q11" s="37">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B231A4-BC20-493A-9F2E-2632555001BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B231A4-BC20-493A-9F2E-2632555001BB}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5684,9 +5780,7 @@
     <col min="10" max="10" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -5736,10 +5830,10 @@
         <v>195</v>
       </c>
       <c r="P1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q1" t="s">
         <v>198</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -5789,9 +5883,6 @@
         <v>6006000</v>
       </c>
       <c r="P2">
-        <v>0.33982920954674833</v>
-      </c>
-      <c r="Q2">
         <v>36682000</v>
       </c>
     </row>
@@ -5842,9 +5933,6 @@
         <v>5975000</v>
       </c>
       <c r="P3">
-        <v>0.28811610863629822</v>
-      </c>
-      <c r="Q3">
         <v>38899000</v>
       </c>
     </row>
@@ -5895,9 +5983,6 @@
         <v>7204000</v>
       </c>
       <c r="P4">
-        <v>0.15777069180646053</v>
-      </c>
-      <c r="Q4">
         <v>42086000</v>
       </c>
     </row>
@@ -5948,9 +6033,6 @@
         <v>6664000</v>
       </c>
       <c r="P5">
-        <v>-0.42251736437018961</v>
-      </c>
-      <c r="Q5">
         <v>43491000</v>
       </c>
     </row>
@@ -6001,9 +6083,6 @@
         <v>9499000</v>
       </c>
       <c r="P6">
-        <v>-0.67769706752757597</v>
-      </c>
-      <c r="Q6">
         <v>41740000</v>
       </c>
     </row>
@@ -6054,9 +6133,6 @@
         <v>8853000</v>
       </c>
       <c r="P7">
-        <v>-0.29418633235004921</v>
-      </c>
-      <c r="Q7">
         <v>52150000</v>
       </c>
     </row>
@@ -6107,9 +6183,6 @@
         <v>6468000</v>
       </c>
       <c r="P8">
-        <v>-0.23179386395894752</v>
-      </c>
-      <c r="Q8">
         <v>39836000</v>
       </c>
     </row>
@@ -6160,9 +6233,6 @@
         <v>5277000</v>
       </c>
       <c r="P9">
-        <v>0.10605095541401277</v>
-      </c>
-      <c r="Q9">
         <v>38436000</v>
       </c>
     </row>
@@ -6213,9 +6283,6 @@
         <v>5485000</v>
       </c>
       <c r="P10">
-        <v>0.10700624760933319</v>
-      </c>
-      <c r="Q10">
         <v>35829000</v>
       </c>
     </row>
@@ -6266,24 +6333,26 @@
         <v>15514000</v>
       </c>
       <c r="P11">
-        <v>-0.5007078810759793</v>
-      </c>
-      <c r="Q11">
         <v>71888000</v>
+      </c>
+      <c r="Q11" s="36">
+        <f>7.25% + 21%</f>
+        <v>0.28249999999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE62E8B-B252-4389-A5F4-D2A4703DD146}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE62E8B-B252-4389-A5F4-D2A4703DD146}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6298,8 +6367,7 @@
     <col min="10" max="10" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -6349,10 +6417,10 @@
         <v>195</v>
       </c>
       <c r="P1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q1" t="s">
         <v>198</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -6402,9 +6470,6 @@
         <v>4774000</v>
       </c>
       <c r="P2">
-        <v>0.16758080313418211</v>
-      </c>
-      <c r="Q2">
         <v>20358999.99999997</v>
       </c>
     </row>
@@ -6455,9 +6520,6 @@
         <v>4148000</v>
       </c>
       <c r="P3">
-        <v>-0.54259686217173697</v>
-      </c>
-      <c r="Q3">
         <v>21901000</v>
       </c>
     </row>
@@ -6508,9 +6570,6 @@
         <v>6063000</v>
       </c>
       <c r="P4">
-        <v>0.1646305125148988</v>
-      </c>
-      <c r="Q4">
         <v>23686000</v>
       </c>
     </row>
@@ -6561,9 +6620,6 @@
         <v>6108000</v>
       </c>
       <c r="P5">
-        <v>0.16824613786836307</v>
-      </c>
-      <c r="Q5">
         <v>28425000</v>
       </c>
     </row>
@@ -6614,9 +6670,6 @@
         <v>6729000</v>
       </c>
       <c r="P6">
-        <v>9.7058123860122025E-2</v>
-      </c>
-      <c r="Q6">
         <v>32090000</v>
       </c>
     </row>
@@ -6667,9 +6720,6 @@
         <v>5866000</v>
       </c>
       <c r="P7">
-        <v>-0.23303784520968296</v>
-      </c>
-      <c r="Q7">
         <v>29148000</v>
       </c>
     </row>
@@ -6720,9 +6770,6 @@
         <v>6471000</v>
       </c>
       <c r="P8">
-        <v>0.22373637264618429</v>
-      </c>
-      <c r="Q8">
         <v>37855000</v>
       </c>
     </row>
@@ -6773,9 +6820,6 @@
         <v>6216000</v>
       </c>
       <c r="P9">
-        <v>8.8089588276924369E-2</v>
-      </c>
-      <c r="Q9">
         <v>31025000</v>
       </c>
     </row>
@@ -6826,9 +6870,6 @@
         <v>7188000</v>
       </c>
       <c r="P10">
-        <v>0.20359453630481661</v>
-      </c>
-      <c r="Q10">
         <v>27909000</v>
       </c>
     </row>
@@ -6879,24 +6920,25 @@
         <v>8293000</v>
       </c>
       <c r="P11">
-        <v>-0.37168439477581794</v>
-      </c>
-      <c r="Q11">
         <v>26348000</v>
+      </c>
+      <c r="Q11" s="37">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80605593-FA81-460E-B498-6BBA7B2DB4BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80605593-FA81-460E-B498-6BBA7B2DB4BD}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6912,8 +6954,7 @@
     <col min="11" max="13" width="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -6963,10 +7004,10 @@
         <v>195</v>
       </c>
       <c r="P1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q1" t="s">
         <v>198</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -7016,9 +7057,6 @@
         <v>1847700</v>
       </c>
       <c r="P2">
-        <v>0.25509307676218373</v>
-      </c>
-      <c r="Q2">
         <v>8021500</v>
       </c>
     </row>
@@ -7069,9 +7107,6 @@
         <v>1654400</v>
       </c>
       <c r="P3">
-        <v>0.15844544095665181</v>
-      </c>
-      <c r="Q3">
         <v>7978500</v>
       </c>
     </row>
@@ -7122,9 +7157,6 @@
         <v>1752400</v>
       </c>
       <c r="P4">
-        <v>0.23246639392168333</v>
-      </c>
-      <c r="Q4">
         <v>10305200</v>
       </c>
     </row>
@@ -7175,9 +7207,6 @@
         <v>2297900</v>
       </c>
       <c r="P5">
-        <v>-12.29250367466928</v>
-      </c>
-      <c r="Q5">
         <v>13647100</v>
       </c>
     </row>
@@ -7228,9 +7257,6 @@
         <v>1748100</v>
       </c>
       <c r="P6">
-        <v>0.13864480198019802</v>
-      </c>
-      <c r="Q6">
         <v>10298600</v>
       </c>
     </row>
@@ -7281,9 +7307,6 @@
         <v>1730400</v>
       </c>
       <c r="P7">
-        <v>-0.36695758799769185</v>
-      </c>
-      <c r="Q7">
         <v>15317199.999999985</v>
       </c>
     </row>
@@ -7334,9 +7357,6 @@
         <v>1303900</v>
       </c>
       <c r="P8">
-        <v>0.16729902965916987</v>
-      </c>
-      <c r="Q8">
         <v>16595300</v>
       </c>
     </row>
@@ -7387,9 +7407,6 @@
         <v>1850700</v>
       </c>
       <c r="P9">
-        <v>0.10280022215454077</v>
-      </c>
-      <c r="Q9">
         <v>16884700</v>
       </c>
     </row>
@@ -7440,9 +7457,6 @@
         <v>1744100</v>
       </c>
       <c r="P10">
-        <v>8.9930822444273639E-2</v>
-      </c>
-      <c r="Q10">
         <v>16238600</v>
       </c>
     </row>
@@ -7493,13 +7507,15 @@
         <v>1549500</v>
       </c>
       <c r="P11">
-        <v>0.25078238302419664</v>
-      </c>
-      <c r="Q11">
         <v>25225300</v>
+      </c>
+      <c r="Q11" s="36">
+        <f>8.5% + 21%</f>
+        <v>0.29499999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More changes to the excel
</commit_message>
<xml_diff>
--- a/FinancialManagement/Pharma_Data.xlsx
+++ b/FinancialManagement/Pharma_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3863360b7313d4a6/Documentos/GitHub/UC3M_Projects/FinancialManagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1306" documentId="13_ncr:1_{9CE7DB7C-C080-4BB2-8A92-1D4A7BD45BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57A87E0C-C66C-4FEE-8C5A-E96DBC1DC92C}"/>
+  <xr:revisionPtr revIDLastSave="1337" documentId="13_ncr:1_{9CE7DB7C-C080-4BB2-8A92-1D4A7BD45BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{892C9AA0-8682-4834-915C-6CBF97F379CE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Search strategy" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="V11" authorId="1" shapeId="0" xr:uid="{446BE28C-59F2-4B47-B53E-DA33B790B7A3}">
+    <comment ref="W11" authorId="1" shapeId="0" xr:uid="{446BE28C-59F2-4B47-B53E-DA33B790B7A3}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="219">
   <si>
     <t>Product name</t>
   </si>
@@ -1131,9 +1131,6 @@
     <t>D/V</t>
   </si>
   <si>
-    <t>La media del ratio D / V fue:</t>
-  </si>
-  <si>
     <t>rd</t>
   </si>
   <si>
@@ -1141,6 +1138,9 @@
   </si>
   <si>
     <t>TS</t>
+  </si>
+  <si>
+    <t>La media del ratio D/V del sector fue:</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1211,12 +1211,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1595,6 +1589,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1617,7 +1612,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2897,39 +2891,39 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'ROCHE HOLDING AG'!$L$2:$L$11</c:f>
+              <c:f>'PFIZER INC'!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>14245272.7067471</c:v>
+                  <c:v>12726000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13931055.8230877</c:v>
+                  <c:v>10329000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13847441.0505295</c:v>
+                  <c:v>9004000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13332307.954073001</c:v>
+                  <c:v>12989000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14998476.864337901</c:v>
+                  <c:v>4062000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18124353.956699401</c:v>
+                  <c:v>12331000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21042896.235466</c:v>
+                  <c:v>7534000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19891531.4739943</c:v>
+                  <c:v>23486000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18928784.081935901</c:v>
+                  <c:v>36237000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18326290.6527519</c:v>
+                  <c:v>-929000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4276,6 +4270,652 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>D/E de las compañías</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>J&amp;J</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'ROCHE HOLDING AG'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'JOHNSON &amp; JOHNSON'!$T$2:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.4092277574088155E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9878855621977348E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.6544961466626408E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2127413963828939E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6622933945440614E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2141680133365416E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5119924296995317E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4942537485751651E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.5870147642978331E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.773837535128035E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B841-41E7-A077-53B576595F0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Roche</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'ROCHE HOLDING AG'!$T$2:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.13560686503433594</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11973428310493527</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13679803642017296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10948038616311</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10976367034938629</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0633131849521247E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0988377845519354E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12221901988273991</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.13005742259858386</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00%">
+                  <c:v>0.17919788584171276</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B841-41E7-A077-53B576595F0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Pfizer</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'PFIZER INC'!$T$2:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.18689991577784967</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19521290032125391</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2135259425344388</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20144344317502844</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16542634951795934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24051442026690081</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1946974932419159</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11596677197770668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.12456790886878939</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00%">
+                  <c:v>0.44222374567794082</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B841-41E7-A077-53B576595F0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Novartis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'NOVARTIS AG'!$T$2:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.0575128891098302E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3508782761580478E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12361983972268509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12856818411971854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14741477711122725</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12150346930271523</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16164114128332377</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14488945988623</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.12824049478859698</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00%">
+                  <c:v>0.11451026466998719</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B841-41E7-A077-53B576595F0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Eli Lilly</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'ELI LILLY AND COMPANY'!$T$2:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.10442551098163294</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5453532396543713E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12691852675956325</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14674544344026691</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4012065920098564E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12138206199670983</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10275140089555157</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3901536803928488E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6714582850026054E-2</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00%">
+                  <c:v>4.5584857836116252E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B841-41E7-A077-53B576595F0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="580336639"/>
+        <c:axId val="580340479"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="580336639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="580340479"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="580340479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="580336639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12805489938757658"/>
+          <c:y val="0.14285724701079031"/>
+          <c:w val="0.1663895450568679"/>
+          <c:h val="0.39062773403324585"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4476,6 +5116,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6638,6 +7318,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7178,6 +8374,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A73A6FCE-9CB5-6D4A-7CA1-3795FB7D9817}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7530,7 +8762,7 @@
     <text xml:space="preserve">7,25% del Estad de Nueva York y 21% federal
 </text>
   </threadedComment>
-  <threadedComment ref="V11" dT="2024-04-19T15:33:46.19" personId="{743F5DB6-1958-42C6-BD5F-77B09807DC6D}" id="{446BE28C-59F2-4B47-B53E-DA33B790B7A3}">
+  <threadedComment ref="W11" dT="2024-04-19T15:33:46.19" personId="{743F5DB6-1958-42C6-BD5F-77B09807DC6D}" id="{446BE28C-59F2-4B47-B53E-DA33B790B7A3}">
     <text xml:space="preserve">Se usó el spread del año anterior porque si se cogía el EBIT de ese año y los intereses nuevos, el ICR seguía siendo &gt; 8 </text>
   </threadedComment>
 </ThreadedComments>
@@ -7572,86 +8804,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="59" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="60"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="59" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="60"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="59" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="60"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="61"/>
     </row>
     <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="59" t="s">
+      <c r="B4" s="53"/>
+      <c r="C4" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="60"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="61"/>
     </row>
     <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="59" t="s">
+      <c r="B5" s="53"/>
+      <c r="C5" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="60"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="61"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="59" t="s">
+      <c r="B6" s="53"/>
+      <c r="C6" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="60"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="61"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="59" t="s">
+      <c r="B7" s="53"/>
+      <c r="C7" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="60"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="61"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="61"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
@@ -7663,10 +8895,10 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="52"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
@@ -7678,10 +8910,10 @@
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="52"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
@@ -7693,10 +8925,10 @@
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="52"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
@@ -7708,10 +8940,10 @@
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="52"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
@@ -7723,10 +8955,10 @@
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="56"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="7" t="s">
         <v>18</v>
       </c>
@@ -7735,17 +8967,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
     </row>
     <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="9" t="s">
         <v>33</v>
       </c>
@@ -7754,22 +8986,22 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -10466,8 +11698,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10557,13 +11789,13 @@
         <v>213</v>
       </c>
       <c r="V1" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="W1" s="26" t="s">
         <v>214</v>
       </c>
       <c r="X1" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
@@ -10629,7 +11861,7 @@
       <c r="U2" s="31"/>
       <c r="V2" s="31"/>
       <c r="W2" s="31">
-        <f>P2/I2</f>
+        <f t="shared" ref="W2:W11" si="0">P2/I2</f>
         <v>6.7391358466454318E-2</v>
       </c>
       <c r="X2" s="32"/>
@@ -10692,13 +11924,13 @@
         <v>2.0042436059181101E-2</v>
       </c>
       <c r="T3" s="31">
-        <f t="shared" ref="T3:T11" si="0">P3/E3</f>
+        <f t="shared" ref="T3:T11" si="1">P3/E3</f>
         <v>6.9878855621977348E-2</v>
       </c>
       <c r="U3" s="31"/>
       <c r="V3" s="31"/>
       <c r="W3" s="31">
-        <f>P3/I3</f>
+        <f t="shared" si="0"/>
         <v>7.4748183658842712E-2</v>
       </c>
       <c r="X3" s="32"/>
@@ -10758,17 +11990,17 @@
       </c>
       <c r="R4" s="31"/>
       <c r="S4" s="31">
-        <f t="shared" ref="S4:S11" si="1">C4/C3 - 1</f>
+        <f t="shared" ref="S4:S11" si="2">C4/C3 - 1</f>
         <v>-1.0288123682361205E-2</v>
       </c>
       <c r="T4" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.6544961466626408E-2</v>
       </c>
       <c r="U4" s="31"/>
       <c r="V4" s="31"/>
       <c r="W4" s="31">
-        <f>P4/I4</f>
+        <f t="shared" si="0"/>
         <v>9.0828285860904787E-2</v>
       </c>
       <c r="X4" s="32"/>
@@ -10827,17 +12059,17 @@
       </c>
       <c r="R5" s="31"/>
       <c r="S5" s="31">
+        <f t="shared" si="2"/>
+        <v>-0.14567298133999829</v>
+      </c>
+      <c r="T5" s="31">
         <f t="shared" si="1"/>
-        <v>-0.14567298133999829</v>
-      </c>
-      <c r="T5" s="31">
-        <f t="shared" si="0"/>
         <v>9.2127413963828939E-2</v>
       </c>
       <c r="U5" s="31"/>
       <c r="V5" s="31"/>
       <c r="W5" s="31">
-        <f>P5/I5</f>
+        <f t="shared" si="0"/>
         <v>8.8296667508711985E-2</v>
       </c>
       <c r="X5" s="32"/>
@@ -10896,17 +12128,17 @@
       </c>
       <c r="R6" s="31"/>
       <c r="S6" s="31">
+        <f t="shared" si="2"/>
+        <v>-6.7819148936170137E-3</v>
+      </c>
+      <c r="T6" s="31">
         <f t="shared" si="1"/>
-        <v>-6.7819148936170137E-3</v>
-      </c>
-      <c r="T6" s="31">
-        <f t="shared" si="0"/>
         <v>8.6622933945440614E-2</v>
       </c>
       <c r="U6" s="31"/>
       <c r="V6" s="31"/>
       <c r="W6" s="31">
-        <f>P6/I6</f>
+        <f t="shared" si="0"/>
         <v>8.412100265130848E-2</v>
       </c>
       <c r="X6" s="32"/>
@@ -10965,11 +12197,11 @@
       </c>
       <c r="R7" s="31"/>
       <c r="S7" s="31">
+        <f t="shared" si="2"/>
+        <v>-4.7027714553488087E-3</v>
+      </c>
+      <c r="T7" s="31">
         <f t="shared" si="1"/>
-        <v>-4.7027714553488087E-3</v>
-      </c>
-      <c r="T7" s="31">
-        <f t="shared" si="0"/>
         <v>7.2141680133365416E-2</v>
       </c>
       <c r="U7" s="31">
@@ -10977,7 +12209,7 @@
       </c>
       <c r="V7" s="31"/>
       <c r="W7" s="31">
-        <f>P7/I7</f>
+        <f t="shared" si="0"/>
         <v>7.0595393792276015E-2</v>
       </c>
       <c r="X7" s="32"/>
@@ -11036,11 +12268,11 @@
       </c>
       <c r="R8" s="31"/>
       <c r="S8" s="31">
+        <f t="shared" si="2"/>
+        <v>6.4014393569975292E-2</v>
+      </c>
+      <c r="T8" s="31">
         <f t="shared" si="1"/>
-        <v>6.4014393569975292E-2</v>
-      </c>
-      <c r="T8" s="31">
-        <f t="shared" si="0"/>
         <v>8.5119924296995317E-2</v>
       </c>
       <c r="U8" s="31">
@@ -11048,7 +12280,7 @@
       </c>
       <c r="V8" s="31"/>
       <c r="W8" s="31">
-        <f>P8/I8</f>
+        <f t="shared" si="0"/>
         <v>8.3097980363037227E-2</v>
       </c>
       <c r="X8" s="32"/>
@@ -11107,11 +12339,11 @@
       </c>
       <c r="R9" s="31"/>
       <c r="S9" s="31">
+        <f t="shared" si="2"/>
+        <v>0.16980625177786912</v>
+      </c>
+      <c r="T9" s="31">
         <f t="shared" si="1"/>
-        <v>0.16980625177786912</v>
-      </c>
-      <c r="T9" s="31">
-        <f t="shared" si="0"/>
         <v>7.4942537485751651E-2</v>
       </c>
       <c r="U9" s="31">
@@ -11119,7 +12351,7 @@
       </c>
       <c r="V9" s="31"/>
       <c r="W9" s="31">
-        <f>P9/I9</f>
+        <f t="shared" si="0"/>
         <v>7.4587617337735293E-2</v>
       </c>
       <c r="X9" s="32"/>
@@ -11179,11 +12411,11 @@
       </c>
       <c r="R10" s="31"/>
       <c r="S10" s="31">
+        <f t="shared" si="2"/>
+        <v>3.75694041041299E-2</v>
+      </c>
+      <c r="T10" s="31">
         <f t="shared" si="1"/>
-        <v>3.75694041041299E-2</v>
-      </c>
-      <c r="T10" s="31">
-        <f t="shared" si="0"/>
         <v>8.5870147642978331E-2</v>
       </c>
       <c r="U10" s="31">
@@ -11191,7 +12423,7 @@
       </c>
       <c r="V10" s="31"/>
       <c r="W10" s="31">
-        <f>P10/I10</f>
+        <f t="shared" si="0"/>
         <v>8.2970613145257735E-2</v>
       </c>
       <c r="X10" s="32"/>
@@ -11253,11 +12485,11 @@
         <v>0.3</v>
       </c>
       <c r="S11" s="31">
+        <f t="shared" si="2"/>
+        <v>-0.1045518462580074</v>
+      </c>
+      <c r="T11" s="31">
         <f t="shared" si="1"/>
-        <v>-0.1045518462580074</v>
-      </c>
-      <c r="T11" s="31">
-        <f t="shared" si="0"/>
         <v>7.773837535128035E-2</v>
       </c>
       <c r="U11" s="31">
@@ -11268,10 +12500,10 @@
         <v>4.53E-2</v>
       </c>
       <c r="W11" s="31">
-        <f>P11/I11</f>
+        <f t="shared" si="0"/>
         <v>7.6440783681797186E-2</v>
       </c>
-      <c r="X11" s="62">
+      <c r="X11" s="52">
         <f>R11*P11</f>
         <v>8799600</v>
       </c>
@@ -11316,10 +12548,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D143F43-DDA8-48B7-AA53-77749AB56B8E}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11337,7 +12569,7 @@
     <col min="18" max="18" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>185</v>
       </c>
@@ -11399,16 +12631,19 @@
         <v>202</v>
       </c>
       <c r="U1" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="X1" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="V1" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>218</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
         <v>2014</v>
       </c>
@@ -11469,10 +12704,14 @@
         <v>0.13560686503433594</v>
       </c>
       <c r="U2" s="34"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32"/>
+      <c r="V2" s="34">
+        <f>P2/I2</f>
+        <v>0.12627639855990955</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>2015</v>
       </c>
@@ -11534,10 +12773,14 @@
         <v>0.11973428310493527</v>
       </c>
       <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="32"/>
+      <c r="V3" s="34">
+        <f t="shared" ref="V3:V11" si="2">P3/I3</f>
+        <v>0.11234466095804965</v>
+      </c>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>2016</v>
       </c>
@@ -11599,10 +12842,14 @@
         <v>0.13679803642017296</v>
       </c>
       <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="32"/>
+      <c r="V4" s="34">
+        <f t="shared" si="2"/>
+        <v>0.12734184797976697</v>
+      </c>
+      <c r="W4" s="31"/>
+      <c r="X4" s="32"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>2017</v>
       </c>
@@ -11664,10 +12911,14 @@
         <v>0.10948038616311</v>
       </c>
       <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="32"/>
+      <c r="V5" s="34">
+        <f t="shared" si="2"/>
+        <v>0.10574827455229649</v>
+      </c>
+      <c r="W5" s="31"/>
+      <c r="X5" s="32"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>2018</v>
       </c>
@@ -11729,10 +12980,14 @@
         <v>0.10976367034938629</v>
       </c>
       <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="32"/>
+      <c r="V6" s="34">
+        <f t="shared" si="2"/>
+        <v>0.10625785940318917</v>
+      </c>
+      <c r="W6" s="31"/>
+      <c r="X6" s="32"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>2019</v>
       </c>
@@ -11796,10 +13051,14 @@
       <c r="U7" s="31">
         <v>6.3E-3</v>
       </c>
-      <c r="V7" s="31"/>
-      <c r="W7" s="32"/>
+      <c r="V7" s="34">
+        <f t="shared" si="2"/>
+        <v>6.9466150511263702E-2</v>
+      </c>
+      <c r="W7" s="31"/>
+      <c r="X7" s="32"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>2020</v>
       </c>
@@ -11863,10 +13122,14 @@
       <c r="U8" s="31">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="V8" s="31"/>
-      <c r="W8" s="32"/>
+      <c r="V8" s="34">
+        <f t="shared" si="2"/>
+        <v>6.9999131535661327E-2</v>
+      </c>
+      <c r="W8" s="31"/>
+      <c r="X8" s="32"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>2021</v>
       </c>
@@ -11930,10 +13193,14 @@
       <c r="U9" s="31">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="V9" s="31"/>
-      <c r="W9" s="32"/>
+      <c r="V9" s="34">
+        <f t="shared" si="2"/>
+        <v>0.11387769929773073</v>
+      </c>
+      <c r="W9" s="31"/>
+      <c r="X9" s="32"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>2022</v>
       </c>
@@ -11997,10 +13264,14 @@
       <c r="U10" s="31">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="V10" s="31"/>
-      <c r="W10" s="32"/>
+      <c r="V10" s="34">
+        <f t="shared" si="2"/>
+        <v>0.12018175896407232</v>
+      </c>
+      <c r="W10" s="31"/>
+      <c r="X10" s="32"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>2023</v>
       </c>
@@ -12066,11 +13337,15 @@
       <c r="U11" s="31">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="V11" s="31">
+      <c r="V11" s="34">
+        <f t="shared" si="2"/>
+        <v>0.16029905535912797</v>
+      </c>
+      <c r="W11" s="31">
         <f>0.7%+U11</f>
         <v>1.2899999999999998E-2</v>
       </c>
-      <c r="W11" s="62">
+      <c r="X11" s="52">
         <f>R11*P11</f>
         <v>5496458.7093829345</v>
       </c>
@@ -12084,17 +13359,18 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B231A4-BC20-493A-9F2E-2632555001BB}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
@@ -12108,7 +13384,7 @@
     <col min="18" max="18" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>185</v>
       </c>
@@ -12170,16 +13446,19 @@
         <v>202</v>
       </c>
       <c r="U1" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="X1" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="V1" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>218</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
         <v>2014</v>
       </c>
@@ -12240,10 +13519,14 @@
         <v>0.18689991577784967</v>
       </c>
       <c r="U2" s="34"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32"/>
+      <c r="V2" s="34">
+        <f>P2/I2</f>
+        <v>0.18636815557271041</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>2015</v>
       </c>
@@ -12305,10 +13588,14 @@
         <v>0.19521290032125391</v>
       </c>
       <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="32"/>
+      <c r="V3" s="34">
+        <f t="shared" ref="V3:V11" si="2">P3/I3</f>
+        <v>0.18103209984088545</v>
+      </c>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>2016</v>
       </c>
@@ -12370,10 +13657,14 @@
         <v>0.2135259425344388</v>
       </c>
       <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="32"/>
+      <c r="V4" s="34">
+        <f t="shared" si="2"/>
+        <v>0.19014515169260268</v>
+      </c>
+      <c r="W4" s="31"/>
+      <c r="X4" s="32"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>2017</v>
       </c>
@@ -12435,10 +13726,14 @@
         <v>0.20144344317502844</v>
       </c>
       <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="32"/>
+      <c r="V5" s="34">
+        <f t="shared" si="2"/>
+        <v>0.1816698341265148</v>
+      </c>
+      <c r="W5" s="31"/>
+      <c r="X5" s="32"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>2018</v>
       </c>
@@ -12500,10 +13795,14 @@
         <v>0.16542634951795934</v>
       </c>
       <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="32"/>
+      <c r="V6" s="34">
+        <f t="shared" si="2"/>
+        <v>0.15165788666573429</v>
+      </c>
+      <c r="W6" s="31"/>
+      <c r="X6" s="32"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>2019</v>
       </c>
@@ -12567,10 +13866,14 @@
       <c r="U7" s="51">
         <v>7.7999999999999996E-3</v>
       </c>
-      <c r="V7" s="31"/>
-      <c r="W7" s="32"/>
+      <c r="V7" s="34">
+        <f t="shared" si="2"/>
+        <v>0.20109441945595102</v>
+      </c>
+      <c r="W7" s="31"/>
+      <c r="X7" s="32"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>2020</v>
       </c>
@@ -12634,10 +13937,14 @@
       <c r="U8" s="51">
         <v>1.18E-2</v>
       </c>
-      <c r="V8" s="31"/>
-      <c r="W8" s="32"/>
+      <c r="V8" s="34">
+        <f t="shared" si="2"/>
+        <v>0.17154453113184001</v>
+      </c>
+      <c r="W8" s="31"/>
+      <c r="X8" s="32"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>2021</v>
       </c>
@@ -12701,10 +14008,14 @@
       <c r="U9" s="51">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="V9" s="31"/>
-      <c r="W9" s="32"/>
+      <c r="V9" s="34">
+        <f t="shared" si="2"/>
+        <v>0.11344519540412487</v>
+      </c>
+      <c r="W9" s="31"/>
+      <c r="X9" s="32"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>2022</v>
       </c>
@@ -12768,10 +14079,14 @@
       <c r="U10" s="51">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="V10" s="31"/>
-      <c r="W10" s="32"/>
+      <c r="V10" s="34">
+        <f t="shared" si="2"/>
+        <v>0.11914276823149215</v>
+      </c>
+      <c r="W10" s="31"/>
+      <c r="X10" s="32"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>2023</v>
       </c>
@@ -12838,11 +14153,15 @@
       <c r="U11" s="51">
         <v>0.2</v>
       </c>
-      <c r="V11" s="51">
+      <c r="V11" s="34">
+        <f t="shared" si="2"/>
+        <v>0.32417284112332706</v>
+      </c>
+      <c r="W11" s="51">
         <f>0.69 %+ 3.94%</f>
         <v>4.6299999999999994E-2</v>
       </c>
-      <c r="W11" s="62">
+      <c r="X11" s="52">
         <f>R11*P11</f>
         <v>20308359.999999996</v>
       </c>
@@ -12856,10 +14175,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE62E8B-B252-4389-A5F4-D2A4703DD146}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="V2" sqref="V2:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12881,7 +14200,7 @@
     <col min="18" max="18" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>185</v>
       </c>
@@ -12943,16 +14262,19 @@
         <v>202</v>
       </c>
       <c r="U1" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="X1" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="V1" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>218</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
         <v>2014</v>
       </c>
@@ -13013,10 +14335,14 @@
         <v>8.0575128891098302E-2</v>
       </c>
       <c r="U2" s="34"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32"/>
+      <c r="V2" s="34">
+        <f>P2/I2</f>
+        <v>7.8447459327470562E-2</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>2015</v>
       </c>
@@ -13078,10 +14404,14 @@
         <v>9.3508782761580478E-2</v>
       </c>
       <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="32"/>
+      <c r="V3" s="34">
+        <f t="shared" ref="V3:V11" si="2">P3/I3</f>
+        <v>8.732097745012371E-2</v>
+      </c>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>2016</v>
       </c>
@@ -13143,10 +14473,14 @@
         <v>0.12361983972268509</v>
       </c>
       <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="32"/>
+      <c r="V4" s="34">
+        <f t="shared" si="2"/>
+        <v>0.11401612298645813</v>
+      </c>
+      <c r="W4" s="31"/>
+      <c r="X4" s="32"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>2017</v>
       </c>
@@ -13208,10 +14542,14 @@
         <v>0.12856818411971854</v>
       </c>
       <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="32"/>
+      <c r="V5" s="34">
+        <f t="shared" si="2"/>
+        <v>0.11840794121928611</v>
+      </c>
+      <c r="W5" s="31"/>
+      <c r="X5" s="32"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>2018</v>
       </c>
@@ -13273,10 +14611,14 @@
         <v>0.14741477711122725</v>
       </c>
       <c r="U6" s="32"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="32"/>
+      <c r="V6" s="34">
+        <f t="shared" si="2"/>
+        <v>0.13717128141401569</v>
+      </c>
+      <c r="W6" s="31"/>
+      <c r="X6" s="32"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>2019</v>
       </c>
@@ -13340,10 +14682,14 @@
       <c r="U7" s="31">
         <v>6.3E-3</v>
       </c>
-      <c r="V7" s="31"/>
-      <c r="W7" s="32"/>
+      <c r="V7" s="34">
+        <f t="shared" si="2"/>
+        <v>0.11310897443427607</v>
+      </c>
+      <c r="W7" s="31"/>
+      <c r="X7" s="32"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>2020</v>
       </c>
@@ -13407,10 +14753,14 @@
       <c r="U8" s="31">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="V8" s="31"/>
-      <c r="W8" s="32"/>
+      <c r="V8" s="34">
+        <f t="shared" si="2"/>
+        <v>0.14523718592576942</v>
+      </c>
+      <c r="W8" s="31"/>
+      <c r="X8" s="32"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>2021</v>
       </c>
@@ -13474,10 +14824,14 @@
       <c r="U9" s="31">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="V9" s="31"/>
-      <c r="W9" s="32"/>
+      <c r="V9" s="34">
+        <f t="shared" si="2"/>
+        <v>0.14301864519450544</v>
+      </c>
+      <c r="W9" s="31"/>
+      <c r="X9" s="32"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>2022</v>
       </c>
@@ -13541,10 +14895,14 @@
       <c r="U10" s="31">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="V10" s="31"/>
-      <c r="W10" s="32"/>
+      <c r="V10" s="34">
+        <f t="shared" si="2"/>
+        <v>0.12304841316809498</v>
+      </c>
+      <c r="W10" s="31"/>
+      <c r="X10" s="32"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>2023</v>
       </c>
@@ -13610,11 +14968,15 @@
       <c r="U11" s="31">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="V11" s="31">
+      <c r="V11" s="34">
+        <f t="shared" si="2"/>
+        <v>0.10871076134474007</v>
+      </c>
+      <c r="W11" s="31">
         <f>U11+0.7%</f>
         <v>1.2899999999999998E-2</v>
       </c>
-      <c r="W11" s="62">
+      <c r="X11" s="52">
         <f>R11*P11</f>
         <v>3952200</v>
       </c>
@@ -13628,10 +14990,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80605593-FA81-460E-B498-6BBA7B2DB4BD}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13653,7 +15015,7 @@
     <col min="18" max="18" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>185</v>
       </c>
@@ -13715,16 +15077,19 @@
         <v>202</v>
       </c>
       <c r="U1" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="X1" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="V1" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>218</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
         <v>2014</v>
       </c>
@@ -13785,10 +15150,14 @@
         <v>0.10442551098163294</v>
       </c>
       <c r="U2" s="34"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32"/>
+      <c r="V2" s="34">
+        <f>P2/I2</f>
+        <v>0.10025619203971817</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>2015</v>
       </c>
@@ -13850,10 +15219,14 @@
         <v>8.5453532396543713E-2</v>
       </c>
       <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="32"/>
+      <c r="V3" s="34">
+        <f t="shared" ref="V3:V11" si="2">P3/I3</f>
+        <v>8.234321225052664E-2</v>
+      </c>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>2016</v>
       </c>
@@ -13915,10 +15288,14 @@
         <v>0.12691852675956325</v>
       </c>
       <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="32"/>
+      <c r="V4" s="34">
+        <f t="shared" si="2"/>
+        <v>0.12058225316880511</v>
+      </c>
+      <c r="W4" s="31"/>
+      <c r="X4" s="32"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>2017</v>
       </c>
@@ -13980,10 +15357,14 @@
         <v>0.14674544344026691</v>
       </c>
       <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="32"/>
+      <c r="V5" s="34">
+        <f t="shared" si="2"/>
+        <v>0.13839263953317557</v>
+      </c>
+      <c r="W5" s="31"/>
+      <c r="X5" s="32"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>2018</v>
       </c>
@@ -14045,10 +15426,14 @@
         <v>8.4012065920098564E-2</v>
       </c>
       <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="32"/>
+      <c r="V6" s="34">
+        <f t="shared" si="2"/>
+        <v>8.2077252712459345E-2</v>
+      </c>
+      <c r="W6" s="31"/>
+      <c r="X6" s="32"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>2019</v>
       </c>
@@ -14112,10 +15497,14 @@
       <c r="U7" s="31">
         <v>6.3E-3</v>
       </c>
-      <c r="V7" s="31"/>
-      <c r="W7" s="32"/>
+      <c r="V7" s="34">
+        <f t="shared" si="2"/>
+        <v>0.11014126241776175</v>
+      </c>
+      <c r="W7" s="31"/>
+      <c r="X7" s="32"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>2020</v>
       </c>
@@ -14179,10 +15568,14 @@
       <c r="U8" s="31">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="V8" s="31"/>
-      <c r="W8" s="32"/>
+      <c r="V8" s="34">
+        <f t="shared" si="2"/>
+        <v>9.51438616674571E-2</v>
+      </c>
+      <c r="W8" s="31"/>
+      <c r="X8" s="32"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>2021</v>
       </c>
@@ -14246,10 +15639,14 @@
       <c r="U9" s="31">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="V9" s="31"/>
-      <c r="W9" s="32"/>
+      <c r="V9" s="34">
+        <f t="shared" si="2"/>
+        <v>6.0910286339327796E-2</v>
+      </c>
+      <c r="W9" s="31"/>
+      <c r="X9" s="32"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>2022</v>
       </c>
@@ -14313,10 +15710,14 @@
       <c r="U10" s="31">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="V10" s="31"/>
-      <c r="W10" s="32"/>
+      <c r="V10" s="34">
+        <f t="shared" si="2"/>
+        <v>4.4902680601561586E-2</v>
+      </c>
+      <c r="W10" s="31"/>
+      <c r="X10" s="32"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>2023</v>
       </c>
@@ -14383,11 +15784,15 @@
       <c r="U11" s="31">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="V11" s="31">
+      <c r="V11" s="34">
+        <f t="shared" si="2"/>
+        <v>4.3819198892550655E-2</v>
+      </c>
+      <c r="W11" s="31">
         <f>3.94%+U11</f>
         <v>4.53E-2</v>
       </c>
-      <c r="W11" s="62">
+      <c r="X11" s="52">
         <f>R11*P11</f>
         <v>7441463.5</v>
       </c>
@@ -14402,8 +15807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1201D640-FACA-47DD-A6E4-D0E6DE97DB38}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14950,7 +16355,7 @@
       <c r="E30" s="45"/>
       <c r="F30" s="37"/>
       <c r="G30" s="49" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H30" s="37"/>
       <c r="I30" s="38"/>
@@ -15169,8 +16574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F4CA64-9DF2-4FC1-BEFD-FEA468E129B0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adding a for-loop to perform sensitivity analysis
</commit_message>
<xml_diff>
--- a/FinancialManagement/Pharma_Data.xlsx
+++ b/FinancialManagement/Pharma_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3863360b7313d4a6/Documentos/GitHub/UC3M_Projects/FinancialManagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1940" documentId="13_ncr:1_{9CE7DB7C-C080-4BB2-8A92-1D4A7BD45BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88B2EF64-D2CE-4C92-931F-F3101F245DF8}"/>
+  <xr:revisionPtr revIDLastSave="1950" documentId="13_ncr:1_{9CE7DB7C-C080-4BB2-8A92-1D4A7BD45BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AFEEE68-B6AE-43BA-BBED-F521C5687149}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Search strategy" sheetId="1" r:id="rId1"/>
@@ -2419,9 +2419,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="13" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="13" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2443,6 +2440,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -9646,86 +9646,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="78" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="79"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="78"/>
     </row>
     <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="78" t="s">
+      <c r="B2" s="76"/>
+      <c r="C2" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="79"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="78"/>
     </row>
     <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="78" t="s">
+      <c r="B3" s="76"/>
+      <c r="C3" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="79"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="78"/>
     </row>
     <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="78" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="79"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="78"/>
     </row>
     <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="78" t="s">
+      <c r="B5" s="76"/>
+      <c r="C5" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="79"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="78"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="78" t="s">
+      <c r="B6" s="76"/>
+      <c r="C6" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="77"/>
-      <c r="E6" s="79"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="78"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="78" t="s">
+      <c r="B7" s="76"/>
+      <c r="C7" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="77"/>
-      <c r="E7" s="79"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="78"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
@@ -9737,10 +9737,10 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="77"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
@@ -9752,10 +9752,10 @@
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="77"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
@@ -9767,10 +9767,10 @@
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="77"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
@@ -9782,10 +9782,10 @@
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="77"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
@@ -9797,10 +9797,10 @@
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="84"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="7" t="s">
         <v>18</v>
       </c>
@@ -9809,17 +9809,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
     </row>
     <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="77"/>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
+      <c r="A15" s="76"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="9" t="s">
         <v>33</v>
       </c>
@@ -9828,22 +9828,22 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="77"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
+      <c r="A16" s="76"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
     </row>
     <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -12540,8 +12540,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13917,7 +13917,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -17196,8 +17196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1201D640-FACA-47DD-A6E4-D0E6DE97DB38}">
   <dimension ref="A1:R1238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17930,7 +17930,7 @@
       </c>
       <c r="E23" s="39"/>
       <c r="F23" s="40"/>
-      <c r="G23" s="75">
+      <c r="G23" s="85">
         <f>SLOPE(R2:R366,Q2:Q366)</f>
         <v>0.33162150375484817</v>
       </c>

</xml_diff>